<commit_message>
'Edit profile' module updated. Project fully updated.
</commit_message>
<xml_diff>
--- a/DigitalResumeBuilder/src/main/resources/user_credentials.xlsx
+++ b/DigitalResumeBuilder/src/main/resources/user_credentials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Repository\DigitalResumeBuilder\DigitalResumeBuilder\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E92BF27-841D-42BF-B629-961240CE5A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325A1DC4-0472-417D-9945-647E8B44A2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIGN UP" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
   <si>
     <t>user</t>
   </si>
@@ -245,13 +245,16 @@
     <t>88</t>
   </si>
   <si>
-    <t>22/04/1992</t>
-  </si>
-  <si>
     <t>8990909090</t>
   </si>
   <si>
-    <t>D:\Eclipse _workspace\DigitalResumeBuilder\src\main\resources\r5.png</t>
+    <t>22/04/2028</t>
+  </si>
+  <si>
+    <t>src\main\resources\sample%20(1).pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thalwar</t>
   </si>
 </sst>
 </file>
@@ -618,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -888,14 +891,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC7D5B6-BCC7-42C2-9B4F-5E2F04921AA0}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.1796875" customWidth="1"/>
-    <col min="2" max="2" width="28.26953125" customWidth="1"/>
+    <col min="2" max="2" width="43.7265625" customWidth="1"/>
     <col min="3" max="3" width="13.81640625" customWidth="1"/>
     <col min="4" max="4" width="18.36328125" customWidth="1"/>
     <col min="5" max="5" width="22.7265625" customWidth="1"/>
@@ -906,7 +909,7 @@
         <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -914,7 +917,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -938,7 +941,7 @@
         <v>54</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -997,7 +1000,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>60</v>
       </c>

</xml_diff>